<commit_message>
Update 241108_MSR_MOP_CTM BOM 정리.xlsx
</commit_message>
<xml_diff>
--- a/241108_MSR_MOP_CTM BOM 정리.xlsx
+++ b/241108_MSR_MOP_CTM BOM 정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/JDS_BU/Git_Hub/GIC_HONGKONG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDE984D-FA2C-1746-BD7D-E0E001942C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8EB534-AE96-4F45-B1FD-E94C0E34B4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7220" yWindow="900" windowWidth="33900" windowHeight="24360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2547,6 +2547,15 @@
     <xf numFmtId="177" fontId="24" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2565,12 +2574,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2581,9 +2584,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="179" fontId="23" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2924,7 +2924,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D143" sqref="D143"/>
+      <selection pane="bottomLeft" activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.3984375" defaultRowHeight="16"/>
@@ -2986,10 +2986,10 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="19">
-      <c r="B3" s="235">
+      <c r="B3" s="236">
         <v>1</v>
       </c>
-      <c r="C3" s="230" t="s">
+      <c r="C3" s="233" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="92"/>
@@ -3006,8 +3006,8 @@
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="2:13" ht="19">
-      <c r="B4" s="234"/>
-      <c r="C4" s="231"/>
+      <c r="B4" s="235"/>
+      <c r="C4" s="226"/>
       <c r="D4" s="12" t="str">
         <f>MOP!D3</f>
         <v>Main Frame</v>
@@ -3038,8 +3038,8 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="2:13" ht="19">
-      <c r="B5" s="234"/>
-      <c r="C5" s="231"/>
+      <c r="B5" s="235"/>
+      <c r="C5" s="226"/>
       <c r="D5" s="12" t="str">
         <f>MOP!D4</f>
         <v>Left Cover</v>
@@ -3070,8 +3070,8 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="2:13" ht="19">
-      <c r="B6" s="234"/>
-      <c r="C6" s="231"/>
+      <c r="B6" s="235"/>
+      <c r="C6" s="226"/>
       <c r="D6" s="12" t="str">
         <f>MOP!D5</f>
         <v>Right Cover</v>
@@ -3102,8 +3102,8 @@
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="2:13" ht="19">
-      <c r="B7" s="234"/>
-      <c r="C7" s="231"/>
+      <c r="B7" s="235"/>
+      <c r="C7" s="226"/>
       <c r="D7" s="12" t="str">
         <f>MOP!D6</f>
         <v>Upper Cover</v>
@@ -3134,8 +3134,8 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="2:13" ht="19">
-      <c r="B8" s="234"/>
-      <c r="C8" s="231"/>
+      <c r="B8" s="235"/>
+      <c r="C8" s="226"/>
       <c r="D8" s="12" t="str">
         <f>MOP!D7</f>
         <v>Lower Cover</v>
@@ -3166,8 +3166,8 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="2:13" ht="19">
-      <c r="B9" s="234"/>
-      <c r="C9" s="231"/>
+      <c r="B9" s="235"/>
+      <c r="C9" s="226"/>
       <c r="D9" s="12" t="str">
         <f>MOP!D8</f>
         <v>Rear Cover</v>
@@ -3198,8 +3198,8 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="2:13" ht="19">
-      <c r="B10" s="234"/>
-      <c r="C10" s="231"/>
+      <c r="B10" s="235"/>
+      <c r="C10" s="226"/>
       <c r="D10" s="12" t="str">
         <f>MOP!D9</f>
         <v>Push Button</v>
@@ -3230,8 +3230,8 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="2:13" ht="19">
-      <c r="B11" s="234"/>
-      <c r="C11" s="231"/>
+      <c r="B11" s="235"/>
+      <c r="C11" s="226"/>
       <c r="D11" s="12" t="str">
         <f>MOP!D10</f>
         <v>Push Button</v>
@@ -3262,8 +3262,8 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="2:13" ht="19">
-      <c r="B12" s="234"/>
-      <c r="C12" s="231"/>
+      <c r="B12" s="235"/>
+      <c r="C12" s="226"/>
       <c r="D12" s="12" t="str">
         <f>MOP!D11</f>
         <v>Push Button</v>
@@ -3294,8 +3294,8 @@
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="2:13" ht="19">
-      <c r="B13" s="234"/>
-      <c r="C13" s="231"/>
+      <c r="B13" s="235"/>
+      <c r="C13" s="226"/>
       <c r="D13" s="110" t="str">
         <f>MOP!D12</f>
         <v>Microphone</v>
@@ -3332,8 +3332,8 @@
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="2:13" ht="38">
-      <c r="B14" s="234"/>
-      <c r="C14" s="231"/>
+      <c r="B14" s="235"/>
+      <c r="C14" s="226"/>
       <c r="D14" s="12" t="str">
         <f>MOP!D13</f>
         <v>LCD</v>
@@ -3367,8 +3367,8 @@
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="2:13" ht="19">
-      <c r="B15" s="234"/>
-      <c r="C15" s="231"/>
+      <c r="B15" s="235"/>
+      <c r="C15" s="226"/>
       <c r="D15" s="12" t="str">
         <f>MOP!D14</f>
         <v>LCD Mount Bracket</v>
@@ -3399,8 +3399,8 @@
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="2:13" ht="19">
-      <c r="B16" s="234"/>
-      <c r="C16" s="231"/>
+      <c r="B16" s="235"/>
+      <c r="C16" s="226"/>
       <c r="D16" s="12" t="str">
         <f>MOP!D15</f>
         <v>LCD Control Board</v>
@@ -3431,8 +3431,8 @@
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="2:13" ht="19">
-      <c r="B17" s="234"/>
-      <c r="C17" s="231"/>
+      <c r="B17" s="235"/>
+      <c r="C17" s="226"/>
       <c r="D17" s="12" t="str">
         <f>MOP!D16</f>
         <v>Main Control Board</v>
@@ -3463,8 +3463,8 @@
       <c r="M17" s="2"/>
     </row>
     <row r="18" spans="2:13" ht="19">
-      <c r="B18" s="234"/>
-      <c r="C18" s="231"/>
+      <c r="B18" s="235"/>
+      <c r="C18" s="226"/>
       <c r="D18" s="12" t="str">
         <f>MOP!D17</f>
         <v>Power Board</v>
@@ -3495,8 +3495,8 @@
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="2:13" ht="19">
-      <c r="B19" s="234"/>
-      <c r="C19" s="231"/>
+      <c r="B19" s="235"/>
+      <c r="C19" s="226"/>
       <c r="D19" s="110" t="str">
         <f>MOP!D18</f>
         <v>3P Connector Male</v>
@@ -3533,8 +3533,8 @@
       <c r="M19" s="2"/>
     </row>
     <row r="20" spans="2:13" ht="19">
-      <c r="B20" s="234"/>
-      <c r="C20" s="231"/>
+      <c r="B20" s="235"/>
+      <c r="C20" s="226"/>
       <c r="D20" s="18" t="str">
         <f>MOP!D19</f>
         <v>3P Connector Female</v>
@@ -3567,8 +3567,8 @@
       </c>
     </row>
     <row r="21" spans="2:13" ht="19">
-      <c r="B21" s="234"/>
-      <c r="C21" s="231"/>
+      <c r="B21" s="235"/>
+      <c r="C21" s="226"/>
       <c r="D21" s="110" t="str">
         <f>MOP!D20</f>
         <v>Locking</v>
@@ -3605,8 +3605,8 @@
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="2:13" ht="19">
-      <c r="B22" s="234"/>
-      <c r="C22" s="231"/>
+      <c r="B22" s="235"/>
+      <c r="C22" s="226"/>
       <c r="D22" s="110" t="str">
         <f>MOP!D21</f>
         <v>4P Connector</v>
@@ -3643,8 +3643,8 @@
       <c r="M22" s="2"/>
     </row>
     <row r="23" spans="2:13" ht="19">
-      <c r="B23" s="234"/>
-      <c r="C23" s="231"/>
+      <c r="B23" s="235"/>
+      <c r="C23" s="226"/>
       <c r="D23" s="110" t="str">
         <f>MOP!D22</f>
         <v>Pin</v>
@@ -3681,8 +3681,8 @@
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="2:13" ht="19">
-      <c r="B24" s="234"/>
-      <c r="C24" s="231"/>
+      <c r="B24" s="235"/>
+      <c r="C24" s="226"/>
       <c r="D24" s="110" t="str">
         <f>MOP!D23</f>
         <v>12P Connector</v>
@@ -3719,8 +3719,8 @@
       <c r="M24" s="2"/>
     </row>
     <row r="25" spans="2:13" ht="19">
-      <c r="B25" s="234"/>
-      <c r="C25" s="231"/>
+      <c r="B25" s="235"/>
+      <c r="C25" s="226"/>
       <c r="D25" s="110" t="str">
         <f>MOP!D24</f>
         <v>Pin</v>
@@ -3757,8 +3757,8 @@
       <c r="M25" s="2"/>
     </row>
     <row r="26" spans="2:13" ht="19">
-      <c r="B26" s="234"/>
-      <c r="C26" s="231"/>
+      <c r="B26" s="235"/>
+      <c r="C26" s="226"/>
       <c r="D26" s="110" t="str">
         <f>MOP!D25</f>
         <v>Cable Clamp</v>
@@ -3795,8 +3795,8 @@
       <c r="M26" s="2"/>
     </row>
     <row r="27" spans="2:13" ht="19">
-      <c r="B27" s="234"/>
-      <c r="C27" s="231"/>
+      <c r="B27" s="235"/>
+      <c r="C27" s="226"/>
       <c r="D27" s="12" t="str">
         <f>MOP!D26</f>
         <v>Name Plate, AL, T1</v>
@@ -3827,8 +3827,8 @@
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="2:13" ht="19">
-      <c r="B28" s="234"/>
-      <c r="C28" s="231"/>
+      <c r="B28" s="235"/>
+      <c r="C28" s="226"/>
       <c r="D28" s="18" t="str">
         <f>MOP!D27</f>
         <v>SPEAKER</v>
@@ -3861,8 +3861,8 @@
       </c>
     </row>
     <row r="29" spans="2:13" ht="18">
-      <c r="B29" s="234"/>
-      <c r="C29" s="231"/>
+      <c r="B29" s="235"/>
+      <c r="C29" s="226"/>
       <c r="D29" s="155"/>
       <c r="E29" s="155"/>
       <c r="F29" s="155"/>
@@ -3875,8 +3875,8 @@
       <c r="M29" s="158"/>
     </row>
     <row r="30" spans="2:13" ht="19">
-      <c r="B30" s="236"/>
-      <c r="C30" s="232"/>
+      <c r="B30" s="237"/>
+      <c r="C30" s="227"/>
       <c r="D30" s="108" t="s">
         <v>172</v>
       </c>
@@ -3902,10 +3902,10 @@
       <c r="M30" s="15"/>
     </row>
     <row r="31" spans="2:13" ht="19">
-      <c r="B31" s="233">
+      <c r="B31" s="234">
         <v>2</v>
       </c>
-      <c r="C31" s="225" t="s">
+      <c r="C31" s="228" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="111"/>
@@ -3922,8 +3922,8 @@
       <c r="M31" s="3"/>
     </row>
     <row r="32" spans="2:13" ht="19">
-      <c r="B32" s="234"/>
-      <c r="C32" s="226"/>
+      <c r="B32" s="235"/>
+      <c r="C32" s="229"/>
       <c r="D32" s="13" t="str">
         <f>MSR!D3</f>
         <v>PWR Board</v>
@@ -3954,8 +3954,8 @@
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="2:13" ht="19">
-      <c r="B33" s="234"/>
-      <c r="C33" s="226"/>
+      <c r="B33" s="235"/>
+      <c r="C33" s="229"/>
       <c r="D33" s="13" t="str">
         <f>MSR!D4</f>
         <v>M_TX Board</v>
@@ -3986,8 +3986,8 @@
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="2:13" ht="19">
-      <c r="B34" s="234"/>
-      <c r="C34" s="226"/>
+      <c r="B34" s="235"/>
+      <c r="C34" s="229"/>
       <c r="D34" s="13" t="str">
         <f>MSR!D5</f>
         <v>Hub Board</v>
@@ -4018,8 +4018,8 @@
       <c r="M34" s="3"/>
     </row>
     <row r="35" spans="2:13" ht="19">
-      <c r="B35" s="234"/>
-      <c r="C35" s="226"/>
+      <c r="B35" s="235"/>
+      <c r="C35" s="229"/>
       <c r="D35" s="13" t="str">
         <f>MSR!D6</f>
         <v>TCIU Board</v>
@@ -4050,8 +4050,8 @@
       <c r="M35" s="3"/>
     </row>
     <row r="36" spans="2:13" ht="19">
-      <c r="B36" s="234"/>
-      <c r="C36" s="226"/>
+      <c r="B36" s="235"/>
+      <c r="C36" s="229"/>
       <c r="D36" s="13" t="str">
         <f>MSR!D7</f>
         <v>PA_PBX Board</v>
@@ -4082,8 +4082,8 @@
       <c r="M36" s="3"/>
     </row>
     <row r="37" spans="2:13" ht="19">
-      <c r="B37" s="234"/>
-      <c r="C37" s="226"/>
+      <c r="B37" s="235"/>
+      <c r="C37" s="229"/>
       <c r="D37" s="13" t="str">
         <f>MSR!D8</f>
         <v>PA_ETX Board</v>
@@ -4114,8 +4114,8 @@
       <c r="M37" s="3"/>
     </row>
     <row r="38" spans="2:13" ht="19">
-      <c r="B38" s="234"/>
-      <c r="C38" s="226"/>
+      <c r="B38" s="235"/>
+      <c r="C38" s="229"/>
       <c r="D38" s="13" t="str">
         <f>MSR!D9</f>
         <v>NVR Board</v>
@@ -4147,8 +4147,8 @@
       <c r="M38" s="3"/>
     </row>
     <row r="39" spans="2:13" ht="38">
-      <c r="B39" s="234"/>
-      <c r="C39" s="226"/>
+      <c r="B39" s="235"/>
+      <c r="C39" s="229"/>
       <c r="D39" s="150" t="str">
         <f>MSR!D10</f>
         <v>CPU
@@ -4180,8 +4180,8 @@
       <c r="M39" s="3"/>
     </row>
     <row r="40" spans="2:13" ht="38">
-      <c r="B40" s="234"/>
-      <c r="C40" s="226"/>
+      <c r="B40" s="235"/>
+      <c r="C40" s="229"/>
       <c r="D40" s="150" t="str">
         <f>MSR!D11</f>
         <v>CPU BRACKET 
@@ -4213,8 +4213,8 @@
       <c r="M40" s="3"/>
     </row>
     <row r="41" spans="2:13" ht="57">
-      <c r="B41" s="234"/>
-      <c r="C41" s="226"/>
+      <c r="B41" s="235"/>
+      <c r="C41" s="229"/>
       <c r="D41" s="151" t="str">
         <f>MSR!D12</f>
         <v>DDR4
@@ -4248,8 +4248,8 @@
       </c>
     </row>
     <row r="42" spans="2:13" ht="19">
-      <c r="B42" s="234"/>
-      <c r="C42" s="226"/>
+      <c r="B42" s="235"/>
+      <c r="C42" s="229"/>
       <c r="D42" s="13" t="str">
         <f>MSR!D13</f>
         <v>SSD Board</v>
@@ -4280,8 +4280,8 @@
       <c r="M42" s="3"/>
     </row>
     <row r="43" spans="2:13" ht="19">
-      <c r="B43" s="234"/>
-      <c r="C43" s="226"/>
+      <c r="B43" s="235"/>
+      <c r="C43" s="229"/>
       <c r="D43" s="116" t="str">
         <f>MSR!D14</f>
         <v>MSR Back Plane</v>
@@ -4318,8 +4318,8 @@
       <c r="M43" s="3"/>
     </row>
     <row r="44" spans="2:13" ht="19">
-      <c r="B44" s="234"/>
-      <c r="C44" s="226"/>
+      <c r="B44" s="235"/>
+      <c r="C44" s="229"/>
       <c r="D44" s="116" t="str">
         <f>MSR!D15</f>
         <v>Frame</v>
@@ -4356,8 +4356,8 @@
       <c r="M44" s="3"/>
     </row>
     <row r="45" spans="2:13" ht="19">
-      <c r="B45" s="234"/>
-      <c r="C45" s="226"/>
+      <c r="B45" s="235"/>
+      <c r="C45" s="229"/>
       <c r="D45" s="13" t="str">
         <f>MSR!D16</f>
         <v>Name Plate, AL, T1</v>
@@ -4388,8 +4388,8 @@
       <c r="M45" s="3"/>
     </row>
     <row r="46" spans="2:13" ht="19">
-      <c r="B46" s="234"/>
-      <c r="C46" s="226"/>
+      <c r="B46" s="235"/>
+      <c r="C46" s="229"/>
       <c r="D46" s="149" t="str">
         <f>MSR!D17</f>
         <v>SSD(2T)</v>
@@ -4422,8 +4422,8 @@
       </c>
     </row>
     <row r="47" spans="2:13" ht="18">
-      <c r="B47" s="234"/>
-      <c r="C47" s="226"/>
+      <c r="B47" s="235"/>
+      <c r="C47" s="229"/>
       <c r="D47" s="155"/>
       <c r="E47" s="155"/>
       <c r="F47" s="155"/>
@@ -4436,8 +4436,8 @@
       <c r="M47" s="158"/>
     </row>
     <row r="48" spans="2:13" ht="19">
-      <c r="B48" s="236"/>
-      <c r="C48" s="227"/>
+      <c r="B48" s="237"/>
+      <c r="C48" s="230"/>
       <c r="D48" s="108" t="s">
         <v>172</v>
       </c>
@@ -4463,10 +4463,10 @@
       <c r="M48" s="15"/>
     </row>
     <row r="49" spans="2:13" ht="19">
-      <c r="B49" s="233">
+      <c r="B49" s="234">
         <v>3</v>
       </c>
-      <c r="C49" s="225" t="s">
+      <c r="C49" s="228" t="s">
         <v>4</v>
       </c>
       <c r="D49" s="111"/>
@@ -4483,8 +4483,8 @@
       <c r="M49" s="3"/>
     </row>
     <row r="50" spans="2:13" ht="19">
-      <c r="B50" s="234"/>
-      <c r="C50" s="226"/>
+      <c r="B50" s="235"/>
+      <c r="C50" s="229"/>
       <c r="D50" s="13" t="str">
         <f>CTM!D3</f>
         <v>Main Frame</v>
@@ -4515,8 +4515,8 @@
       <c r="M50" s="3"/>
     </row>
     <row r="51" spans="2:13" ht="19">
-      <c r="B51" s="234"/>
-      <c r="C51" s="226"/>
+      <c r="B51" s="235"/>
+      <c r="C51" s="229"/>
       <c r="D51" s="13" t="str">
         <f>CTM!D4</f>
         <v>Lower Cover</v>
@@ -4547,8 +4547,8 @@
       <c r="M51" s="3"/>
     </row>
     <row r="52" spans="2:13" ht="19">
-      <c r="B52" s="234"/>
-      <c r="C52" s="226"/>
+      <c r="B52" s="235"/>
+      <c r="C52" s="229"/>
       <c r="D52" s="13" t="str">
         <f>CTM!D5</f>
         <v>Rear Cover</v>
@@ -4579,8 +4579,8 @@
       <c r="M52" s="3"/>
     </row>
     <row r="53" spans="2:13" ht="19">
-      <c r="B53" s="234"/>
-      <c r="C53" s="226"/>
+      <c r="B53" s="235"/>
+      <c r="C53" s="229"/>
       <c r="D53" s="116" t="str">
         <f>CTM!D6</f>
         <v>10.4" LCD</v>
@@ -4619,8 +4619,8 @@
       </c>
     </row>
     <row r="54" spans="2:13" ht="19">
-      <c r="B54" s="234"/>
-      <c r="C54" s="226"/>
+      <c r="B54" s="235"/>
+      <c r="C54" s="229"/>
       <c r="D54" s="13" t="str">
         <f>CTM!D7</f>
         <v>Control Board Bracket</v>
@@ -4650,8 +4650,8 @@
       <c r="M54" s="3"/>
     </row>
     <row r="55" spans="2:13" ht="19">
-      <c r="B55" s="234"/>
-      <c r="C55" s="226"/>
+      <c r="B55" s="235"/>
+      <c r="C55" s="229"/>
       <c r="D55" s="13" t="str">
         <f>CTM!D8</f>
         <v>Control Board</v>
@@ -4681,8 +4681,8 @@
       <c r="M55" s="3"/>
     </row>
     <row r="56" spans="2:13" ht="19">
-      <c r="B56" s="234"/>
-      <c r="C56" s="226"/>
+      <c r="B56" s="235"/>
+      <c r="C56" s="229"/>
       <c r="D56" s="150" t="str">
         <f>CTM!D9</f>
         <v xml:space="preserve">CPU TCA3/i-E3845 </v>
@@ -4721,8 +4721,8 @@
       </c>
     </row>
     <row r="57" spans="2:13" ht="19">
-      <c r="B57" s="234"/>
-      <c r="C57" s="226"/>
+      <c r="B57" s="235"/>
+      <c r="C57" s="229"/>
       <c r="D57" s="150" t="str">
         <f>CTM!D10</f>
         <v xml:space="preserve">CPU BRACKET TCA3/CSP-B </v>
@@ -4761,8 +4761,8 @@
       </c>
     </row>
     <row r="58" spans="2:13" ht="57">
-      <c r="B58" s="234"/>
-      <c r="C58" s="226"/>
+      <c r="B58" s="235"/>
+      <c r="C58" s="229"/>
       <c r="D58" s="151" t="str">
         <f>CTM!D11</f>
         <v>DDR4
@@ -4796,8 +4796,8 @@
       </c>
     </row>
     <row r="59" spans="2:13" ht="19">
-      <c r="B59" s="234"/>
-      <c r="C59" s="226"/>
+      <c r="B59" s="235"/>
+      <c r="C59" s="229"/>
       <c r="D59" s="13" t="str">
         <f>CTM!D12</f>
         <v>Power Board</v>
@@ -4828,8 +4828,8 @@
       <c r="M59" s="3"/>
     </row>
     <row r="60" spans="2:13" ht="19">
-      <c r="B60" s="234"/>
-      <c r="C60" s="226"/>
+      <c r="B60" s="235"/>
+      <c r="C60" s="229"/>
       <c r="D60" s="116" t="str">
         <f>CTM!D13</f>
         <v>3P Connector</v>
@@ -4866,8 +4866,8 @@
       <c r="M60" s="16"/>
     </row>
     <row r="61" spans="2:13" ht="19">
-      <c r="B61" s="234"/>
-      <c r="C61" s="226"/>
+      <c r="B61" s="235"/>
+      <c r="C61" s="229"/>
       <c r="D61" s="116" t="str">
         <f>CTM!D14</f>
         <v>Locking</v>
@@ -4904,8 +4904,8 @@
       <c r="M61" s="16"/>
     </row>
     <row r="62" spans="2:13" ht="19">
-      <c r="B62" s="234"/>
-      <c r="C62" s="226"/>
+      <c r="B62" s="235"/>
+      <c r="C62" s="229"/>
       <c r="D62" s="116" t="str">
         <f>CTM!D15</f>
         <v>4P Connector</v>
@@ -4942,8 +4942,8 @@
       <c r="M62" s="16"/>
     </row>
     <row r="63" spans="2:13" ht="19">
-      <c r="B63" s="234"/>
-      <c r="C63" s="226"/>
+      <c r="B63" s="235"/>
+      <c r="C63" s="229"/>
       <c r="D63" s="116" t="str">
         <f>CTM!D16</f>
         <v>Pin</v>
@@ -4980,8 +4980,8 @@
       <c r="M63" s="16"/>
     </row>
     <row r="64" spans="2:13" ht="19">
-      <c r="B64" s="234"/>
-      <c r="C64" s="226"/>
+      <c r="B64" s="235"/>
+      <c r="C64" s="229"/>
       <c r="D64" s="116" t="str">
         <f>CTM!D17</f>
         <v>Cable Gland</v>
@@ -5018,8 +5018,8 @@
       <c r="M64" s="16"/>
     </row>
     <row r="65" spans="2:13" ht="19">
-      <c r="B65" s="234"/>
-      <c r="C65" s="226"/>
+      <c r="B65" s="235"/>
+      <c r="C65" s="229"/>
       <c r="D65" s="149" t="str">
         <f>CTM!D18</f>
         <v>USB Adapter</v>
@@ -5052,8 +5052,8 @@
       </c>
     </row>
     <row r="66" spans="2:13" ht="19">
-      <c r="B66" s="234"/>
-      <c r="C66" s="226"/>
+      <c r="B66" s="235"/>
+      <c r="C66" s="229"/>
       <c r="D66" s="13" t="str">
         <f>CTM!D19</f>
         <v>Name Plate</v>
@@ -5084,8 +5084,8 @@
       <c r="M66" s="3"/>
     </row>
     <row r="67" spans="2:13" ht="18">
-      <c r="B67" s="234"/>
-      <c r="C67" s="226"/>
+      <c r="B67" s="235"/>
+      <c r="C67" s="229"/>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
@@ -5098,8 +5098,8 @@
       <c r="M67" s="2"/>
     </row>
     <row r="68" spans="2:13" ht="19">
-      <c r="B68" s="236"/>
-      <c r="C68" s="227"/>
+      <c r="B68" s="237"/>
+      <c r="C68" s="230"/>
       <c r="D68" s="108" t="s">
         <v>172</v>
       </c>
@@ -5125,8 +5125,8 @@
       <c r="M68" s="15"/>
     </row>
     <row r="69" spans="2:13" ht="18">
-      <c r="B69" s="233"/>
-      <c r="C69" s="225"/>
+      <c r="B69" s="234"/>
+      <c r="C69" s="228"/>
       <c r="D69" s="111"/>
       <c r="E69" s="112"/>
       <c r="F69" s="95"/>
@@ -5139,8 +5139,8 @@
       <c r="M69" s="3"/>
     </row>
     <row r="70" spans="2:13" ht="18">
-      <c r="B70" s="234"/>
-      <c r="C70" s="226"/>
+      <c r="B70" s="235"/>
+      <c r="C70" s="229"/>
       <c r="D70" s="120"/>
       <c r="E70" s="120"/>
       <c r="F70" s="120"/>
@@ -5153,8 +5153,8 @@
       <c r="M70" s="3"/>
     </row>
     <row r="71" spans="2:13" ht="18">
-      <c r="B71" s="234"/>
-      <c r="C71" s="226"/>
+      <c r="B71" s="235"/>
+      <c r="C71" s="229"/>
       <c r="D71" s="120"/>
       <c r="E71" s="120"/>
       <c r="F71" s="120"/>
@@ -5167,8 +5167,8 @@
       <c r="M71" s="3"/>
     </row>
     <row r="72" spans="2:13" ht="18">
-      <c r="B72" s="234"/>
-      <c r="C72" s="226"/>
+      <c r="B72" s="235"/>
+      <c r="C72" s="229"/>
       <c r="D72" s="120"/>
       <c r="E72" s="120"/>
       <c r="F72" s="120"/>
@@ -5181,8 +5181,8 @@
       <c r="M72" s="3"/>
     </row>
     <row r="73" spans="2:13" ht="18">
-      <c r="B73" s="234"/>
-      <c r="C73" s="226"/>
+      <c r="B73" s="235"/>
+      <c r="C73" s="229"/>
       <c r="D73" s="120"/>
       <c r="E73" s="120"/>
       <c r="F73" s="120"/>
@@ -5195,8 +5195,8 @@
       <c r="M73" s="3"/>
     </row>
     <row r="74" spans="2:13" ht="18">
-      <c r="B74" s="234"/>
-      <c r="C74" s="226"/>
+      <c r="B74" s="235"/>
+      <c r="C74" s="229"/>
       <c r="D74" s="154"/>
       <c r="E74" s="154"/>
       <c r="F74" s="154"/>
@@ -5209,8 +5209,8 @@
       <c r="M74" s="3"/>
     </row>
     <row r="75" spans="2:13" ht="18">
-      <c r="B75" s="234"/>
-      <c r="C75" s="226"/>
+      <c r="B75" s="235"/>
+      <c r="C75" s="229"/>
       <c r="D75" s="154"/>
       <c r="E75" s="154"/>
       <c r="F75" s="154"/>
@@ -5223,8 +5223,8 @@
       <c r="M75" s="3"/>
     </row>
     <row r="76" spans="2:13" ht="18">
-      <c r="B76" s="234"/>
-      <c r="C76" s="226"/>
+      <c r="B76" s="235"/>
+      <c r="C76" s="229"/>
       <c r="D76" s="120"/>
       <c r="E76" s="120"/>
       <c r="F76" s="120"/>
@@ -5237,8 +5237,8 @@
       <c r="M76" s="3"/>
     </row>
     <row r="77" spans="2:13" ht="18">
-      <c r="B77" s="234"/>
-      <c r="C77" s="226"/>
+      <c r="B77" s="235"/>
+      <c r="C77" s="229"/>
       <c r="D77" s="120"/>
       <c r="E77" s="120"/>
       <c r="F77" s="120"/>
@@ -5251,8 +5251,8 @@
       <c r="M77" s="3"/>
     </row>
     <row r="78" spans="2:13" ht="18">
-      <c r="B78" s="234"/>
-      <c r="C78" s="226"/>
+      <c r="B78" s="235"/>
+      <c r="C78" s="229"/>
       <c r="D78" s="120"/>
       <c r="E78" s="120"/>
       <c r="F78" s="120"/>
@@ -5265,8 +5265,8 @@
       <c r="M78" s="3"/>
     </row>
     <row r="79" spans="2:13" ht="18">
-      <c r="B79" s="234"/>
-      <c r="C79" s="226"/>
+      <c r="B79" s="235"/>
+      <c r="C79" s="229"/>
       <c r="D79" s="120"/>
       <c r="E79" s="120"/>
       <c r="F79" s="120"/>
@@ -5279,8 +5279,8 @@
       <c r="M79" s="3"/>
     </row>
     <row r="80" spans="2:13" ht="18">
-      <c r="B80" s="234"/>
-      <c r="C80" s="226"/>
+      <c r="B80" s="235"/>
+      <c r="C80" s="229"/>
       <c r="D80" s="120"/>
       <c r="E80" s="120"/>
       <c r="F80" s="120"/>
@@ -5293,8 +5293,8 @@
       <c r="M80" s="3"/>
     </row>
     <row r="81" spans="2:13" ht="18">
-      <c r="B81" s="234"/>
-      <c r="C81" s="226"/>
+      <c r="B81" s="235"/>
+      <c r="C81" s="229"/>
       <c r="D81" s="120"/>
       <c r="E81" s="120"/>
       <c r="F81" s="120"/>
@@ -5307,8 +5307,8 @@
       <c r="M81" s="3"/>
     </row>
     <row r="82" spans="2:13" ht="18">
-      <c r="B82" s="234"/>
-      <c r="C82" s="226"/>
+      <c r="B82" s="235"/>
+      <c r="C82" s="229"/>
       <c r="D82" s="120"/>
       <c r="E82" s="120"/>
       <c r="F82" s="120"/>
@@ -5321,8 +5321,8 @@
       <c r="M82" s="3"/>
     </row>
     <row r="83" spans="2:13" ht="18">
-      <c r="B83" s="234"/>
-      <c r="C83" s="226"/>
+      <c r="B83" s="235"/>
+      <c r="C83" s="229"/>
       <c r="D83" s="120"/>
       <c r="E83" s="120"/>
       <c r="F83" s="120"/>
@@ -5335,8 +5335,8 @@
       <c r="M83" s="3"/>
     </row>
     <row r="84" spans="2:13" ht="18">
-      <c r="B84" s="234"/>
-      <c r="C84" s="226"/>
+      <c r="B84" s="235"/>
+      <c r="C84" s="229"/>
       <c r="D84" s="154"/>
       <c r="E84" s="154"/>
       <c r="F84" s="154"/>
@@ -5349,8 +5349,8 @@
       <c r="M84" s="3"/>
     </row>
     <row r="85" spans="2:13" ht="18">
-      <c r="B85" s="234"/>
-      <c r="C85" s="226"/>
+      <c r="B85" s="235"/>
+      <c r="C85" s="229"/>
       <c r="D85" s="154"/>
       <c r="E85" s="154"/>
       <c r="F85" s="154"/>
@@ -5363,8 +5363,8 @@
       <c r="M85" s="3"/>
     </row>
     <row r="86" spans="2:13" ht="18">
-      <c r="B86" s="234"/>
-      <c r="C86" s="226"/>
+      <c r="B86" s="235"/>
+      <c r="C86" s="229"/>
       <c r="D86" s="105"/>
       <c r="E86" s="105"/>
       <c r="F86" s="105"/>
@@ -5377,8 +5377,8 @@
       <c r="M86" s="2"/>
     </row>
     <row r="87" spans="2:13" ht="18">
-      <c r="B87" s="236"/>
-      <c r="C87" s="227"/>
+      <c r="B87" s="237"/>
+      <c r="C87" s="230"/>
       <c r="D87" s="108"/>
       <c r="E87" s="108"/>
       <c r="F87" s="109"/>
@@ -5391,8 +5391,8 @@
       <c r="M87" s="2"/>
     </row>
     <row r="88" spans="2:13" ht="18">
-      <c r="B88" s="233"/>
-      <c r="C88" s="225"/>
+      <c r="B88" s="234"/>
+      <c r="C88" s="228"/>
       <c r="D88" s="111"/>
       <c r="E88" s="112"/>
       <c r="F88" s="95"/>
@@ -5405,8 +5405,8 @@
       <c r="M88" s="3"/>
     </row>
     <row r="89" spans="2:13" ht="18">
-      <c r="B89" s="234"/>
-      <c r="C89" s="226"/>
+      <c r="B89" s="235"/>
+      <c r="C89" s="229"/>
       <c r="D89" s="120"/>
       <c r="E89" s="120"/>
       <c r="F89" s="120"/>
@@ -5419,8 +5419,8 @@
       <c r="M89" s="3"/>
     </row>
     <row r="90" spans="2:13" ht="18">
-      <c r="B90" s="234"/>
-      <c r="C90" s="226"/>
+      <c r="B90" s="235"/>
+      <c r="C90" s="229"/>
       <c r="D90" s="120"/>
       <c r="E90" s="120"/>
       <c r="F90" s="120"/>
@@ -5433,8 +5433,8 @@
       <c r="M90" s="3"/>
     </row>
     <row r="91" spans="2:13" ht="18">
-      <c r="B91" s="234"/>
-      <c r="C91" s="226"/>
+      <c r="B91" s="235"/>
+      <c r="C91" s="229"/>
       <c r="D91" s="120"/>
       <c r="E91" s="120"/>
       <c r="F91" s="120"/>
@@ -5447,8 +5447,8 @@
       <c r="M91" s="3"/>
     </row>
     <row r="92" spans="2:13" ht="18">
-      <c r="B92" s="234"/>
-      <c r="C92" s="226"/>
+      <c r="B92" s="235"/>
+      <c r="C92" s="229"/>
       <c r="D92" s="120"/>
       <c r="E92" s="120"/>
       <c r="F92" s="120"/>
@@ -5461,8 +5461,8 @@
       <c r="M92" s="9"/>
     </row>
     <row r="93" spans="2:13" ht="18">
-      <c r="B93" s="234"/>
-      <c r="C93" s="226"/>
+      <c r="B93" s="235"/>
+      <c r="C93" s="229"/>
       <c r="D93" s="120"/>
       <c r="E93" s="120"/>
       <c r="F93" s="120"/>
@@ -5475,8 +5475,8 @@
       <c r="M93" s="3"/>
     </row>
     <row r="94" spans="2:13" ht="18">
-      <c r="B94" s="234"/>
-      <c r="C94" s="226"/>
+      <c r="B94" s="235"/>
+      <c r="C94" s="229"/>
       <c r="D94" s="120"/>
       <c r="E94" s="120"/>
       <c r="F94" s="120"/>
@@ -5489,8 +5489,8 @@
       <c r="M94" s="3"/>
     </row>
     <row r="95" spans="2:13" ht="18">
-      <c r="B95" s="234"/>
-      <c r="C95" s="226"/>
+      <c r="B95" s="235"/>
+      <c r="C95" s="229"/>
       <c r="D95" s="154"/>
       <c r="E95" s="154"/>
       <c r="F95" s="154"/>
@@ -5503,8 +5503,8 @@
       <c r="M95" s="3"/>
     </row>
     <row r="96" spans="2:13" ht="18">
-      <c r="B96" s="234"/>
-      <c r="C96" s="226"/>
+      <c r="B96" s="235"/>
+      <c r="C96" s="229"/>
       <c r="D96" s="154"/>
       <c r="E96" s="154"/>
       <c r="F96" s="154"/>
@@ -5517,8 +5517,8 @@
       <c r="M96" s="3"/>
     </row>
     <row r="97" spans="2:13" ht="18">
-      <c r="B97" s="234"/>
-      <c r="C97" s="226"/>
+      <c r="B97" s="235"/>
+      <c r="C97" s="229"/>
       <c r="D97" s="120"/>
       <c r="E97" s="120"/>
       <c r="F97" s="120"/>
@@ -5531,8 +5531,8 @@
       <c r="M97" s="3"/>
     </row>
     <row r="98" spans="2:13" ht="18">
-      <c r="B98" s="234"/>
-      <c r="C98" s="226"/>
+      <c r="B98" s="235"/>
+      <c r="C98" s="229"/>
       <c r="D98" s="120"/>
       <c r="E98" s="120"/>
       <c r="F98" s="120"/>
@@ -5545,8 +5545,8 @@
       <c r="M98" s="3"/>
     </row>
     <row r="99" spans="2:13" ht="18">
-      <c r="B99" s="234"/>
-      <c r="C99" s="226"/>
+      <c r="B99" s="235"/>
+      <c r="C99" s="229"/>
       <c r="D99" s="120"/>
       <c r="E99" s="120"/>
       <c r="F99" s="120"/>
@@ -5559,8 +5559,8 @@
       <c r="M99" s="3"/>
     </row>
     <row r="100" spans="2:13" ht="18">
-      <c r="B100" s="234"/>
-      <c r="C100" s="226"/>
+      <c r="B100" s="235"/>
+      <c r="C100" s="229"/>
       <c r="D100" s="120"/>
       <c r="E100" s="120"/>
       <c r="F100" s="120"/>
@@ -5573,8 +5573,8 @@
       <c r="M100" s="3"/>
     </row>
     <row r="101" spans="2:13" ht="18">
-      <c r="B101" s="234"/>
-      <c r="C101" s="226"/>
+      <c r="B101" s="235"/>
+      <c r="C101" s="229"/>
       <c r="D101" s="120"/>
       <c r="E101" s="120"/>
       <c r="F101" s="120"/>
@@ -5587,8 +5587,8 @@
       <c r="M101" s="3"/>
     </row>
     <row r="102" spans="2:13" ht="18">
-      <c r="B102" s="234"/>
-      <c r="C102" s="226"/>
+      <c r="B102" s="235"/>
+      <c r="C102" s="229"/>
       <c r="D102" s="120"/>
       <c r="E102" s="120"/>
       <c r="F102" s="120"/>
@@ -5601,8 +5601,8 @@
       <c r="M102" s="3"/>
     </row>
     <row r="103" spans="2:13" ht="18">
-      <c r="B103" s="234"/>
-      <c r="C103" s="226"/>
+      <c r="B103" s="235"/>
+      <c r="C103" s="229"/>
       <c r="D103" s="120"/>
       <c r="E103" s="120"/>
       <c r="F103" s="120"/>
@@ -5615,8 +5615,8 @@
       <c r="M103" s="3"/>
     </row>
     <row r="104" spans="2:13" ht="18">
-      <c r="B104" s="234"/>
-      <c r="C104" s="226"/>
+      <c r="B104" s="235"/>
+      <c r="C104" s="229"/>
       <c r="D104" s="154"/>
       <c r="E104" s="154"/>
       <c r="F104" s="154"/>
@@ -5629,8 +5629,8 @@
       <c r="M104" s="3"/>
     </row>
     <row r="105" spans="2:13" ht="18">
-      <c r="B105" s="234"/>
-      <c r="C105" s="226"/>
+      <c r="B105" s="235"/>
+      <c r="C105" s="229"/>
       <c r="D105" s="120"/>
       <c r="E105" s="120"/>
       <c r="F105" s="120"/>
@@ -5643,8 +5643,8 @@
       <c r="M105" s="2"/>
     </row>
     <row r="106" spans="2:13" ht="18">
-      <c r="B106" s="234"/>
-      <c r="C106" s="226"/>
+      <c r="B106" s="235"/>
+      <c r="C106" s="229"/>
       <c r="D106" s="105"/>
       <c r="E106" s="105"/>
       <c r="F106" s="105"/>
@@ -5657,8 +5657,8 @@
       <c r="M106" s="2"/>
     </row>
     <row r="107" spans="2:13" ht="18">
-      <c r="B107" s="236"/>
-      <c r="C107" s="227"/>
+      <c r="B107" s="237"/>
+      <c r="C107" s="230"/>
       <c r="D107" s="108"/>
       <c r="E107" s="108"/>
       <c r="F107" s="109"/>
@@ -5671,8 +5671,8 @@
       <c r="M107" s="2"/>
     </row>
     <row r="108" spans="2:13" ht="18">
-      <c r="B108" s="233"/>
-      <c r="C108" s="225"/>
+      <c r="B108" s="234"/>
+      <c r="C108" s="228"/>
       <c r="D108" s="111"/>
       <c r="E108" s="112"/>
       <c r="F108" s="95"/>
@@ -5685,8 +5685,8 @@
       <c r="M108" s="3"/>
     </row>
     <row r="109" spans="2:13" ht="18">
-      <c r="B109" s="234"/>
-      <c r="C109" s="226"/>
+      <c r="B109" s="235"/>
+      <c r="C109" s="229"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
       <c r="F109" s="13"/>
@@ -5699,8 +5699,8 @@
       <c r="M109" s="3"/>
     </row>
     <row r="110" spans="2:13" ht="18">
-      <c r="B110" s="234"/>
-      <c r="C110" s="226"/>
+      <c r="B110" s="235"/>
+      <c r="C110" s="229"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
       <c r="F110" s="13"/>
@@ -5713,8 +5713,8 @@
       <c r="M110" s="3"/>
     </row>
     <row r="111" spans="2:13" ht="18">
-      <c r="B111" s="234"/>
-      <c r="C111" s="226"/>
+      <c r="B111" s="235"/>
+      <c r="C111" s="229"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
       <c r="F111" s="13"/>
@@ -5727,8 +5727,8 @@
       <c r="M111" s="3"/>
     </row>
     <row r="112" spans="2:13" ht="18">
-      <c r="B112" s="234"/>
-      <c r="C112" s="226"/>
+      <c r="B112" s="235"/>
+      <c r="C112" s="229"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
       <c r="F112" s="13"/>
@@ -5741,8 +5741,8 @@
       <c r="M112" s="3"/>
     </row>
     <row r="113" spans="2:13" ht="18">
-      <c r="B113" s="234"/>
-      <c r="C113" s="226"/>
+      <c r="B113" s="235"/>
+      <c r="C113" s="229"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
       <c r="F113" s="13"/>
@@ -5755,8 +5755,8 @@
       <c r="M113" s="3"/>
     </row>
     <row r="114" spans="2:13" ht="18">
-      <c r="B114" s="234"/>
-      <c r="C114" s="226"/>
+      <c r="B114" s="235"/>
+      <c r="C114" s="229"/>
       <c r="D114" s="116"/>
       <c r="E114" s="116"/>
       <c r="F114" s="116"/>
@@ -5769,8 +5769,8 @@
       <c r="M114" s="3"/>
     </row>
     <row r="115" spans="2:13" ht="18">
-      <c r="B115" s="234"/>
-      <c r="C115" s="226"/>
+      <c r="B115" s="235"/>
+      <c r="C115" s="229"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
       <c r="F115" s="13"/>
@@ -5783,8 +5783,8 @@
       <c r="M115" s="3"/>
     </row>
     <row r="116" spans="2:13" ht="18">
-      <c r="B116" s="234"/>
-      <c r="C116" s="226"/>
+      <c r="B116" s="235"/>
+      <c r="C116" s="229"/>
       <c r="D116" s="116"/>
       <c r="E116" s="116"/>
       <c r="F116" s="116"/>
@@ -5797,8 +5797,8 @@
       <c r="M116" s="3"/>
     </row>
     <row r="117" spans="2:13" ht="18">
-      <c r="B117" s="234"/>
-      <c r="C117" s="226"/>
+      <c r="B117" s="235"/>
+      <c r="C117" s="229"/>
       <c r="D117" s="116"/>
       <c r="E117" s="116"/>
       <c r="F117" s="116"/>
@@ -5811,8 +5811,8 @@
       <c r="M117" s="3"/>
     </row>
     <row r="118" spans="2:13" ht="18">
-      <c r="B118" s="234"/>
-      <c r="C118" s="226"/>
+      <c r="B118" s="235"/>
+      <c r="C118" s="229"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
       <c r="F118" s="13"/>
@@ -5825,8 +5825,8 @@
       <c r="M118" s="3"/>
     </row>
     <row r="119" spans="2:13" ht="18">
-      <c r="B119" s="234"/>
-      <c r="C119" s="226"/>
+      <c r="B119" s="235"/>
+      <c r="C119" s="229"/>
       <c r="D119" s="12"/>
       <c r="E119" s="12"/>
       <c r="F119" s="12"/>
@@ -5839,8 +5839,8 @@
       <c r="M119" s="2"/>
     </row>
     <row r="120" spans="2:13" ht="18">
-      <c r="B120" s="236"/>
-      <c r="C120" s="227"/>
+      <c r="B120" s="237"/>
+      <c r="C120" s="230"/>
       <c r="D120" s="108"/>
       <c r="E120" s="108"/>
       <c r="F120" s="109"/>
@@ -5853,8 +5853,8 @@
       <c r="M120" s="2"/>
     </row>
     <row r="121" spans="2:13" ht="18">
-      <c r="B121" s="233"/>
-      <c r="C121" s="237"/>
+      <c r="B121" s="234"/>
+      <c r="C121" s="225"/>
       <c r="D121" s="111"/>
       <c r="E121" s="112"/>
       <c r="F121" s="95"/>
@@ -5867,8 +5867,8 @@
       <c r="M121" s="3"/>
     </row>
     <row r="122" spans="2:13" ht="18">
-      <c r="B122" s="234"/>
-      <c r="C122" s="231"/>
+      <c r="B122" s="235"/>
+      <c r="C122" s="226"/>
       <c r="D122" s="120"/>
       <c r="E122" s="120"/>
       <c r="F122" s="120"/>
@@ -5881,8 +5881,8 @@
       <c r="M122" s="4"/>
     </row>
     <row r="123" spans="2:13" ht="18">
-      <c r="B123" s="234"/>
-      <c r="C123" s="231"/>
+      <c r="B123" s="235"/>
+      <c r="C123" s="226"/>
       <c r="D123" s="120"/>
       <c r="E123" s="120"/>
       <c r="F123" s="120"/>
@@ -5895,8 +5895,8 @@
       <c r="M123" s="4"/>
     </row>
     <row r="124" spans="2:13" ht="18">
-      <c r="B124" s="234"/>
-      <c r="C124" s="231"/>
+      <c r="B124" s="235"/>
+      <c r="C124" s="226"/>
       <c r="D124" s="120"/>
       <c r="E124" s="120"/>
       <c r="F124" s="120"/>
@@ -5909,8 +5909,8 @@
       <c r="M124" s="4"/>
     </row>
     <row r="125" spans="2:13" ht="18">
-      <c r="B125" s="234"/>
-      <c r="C125" s="231"/>
+      <c r="B125" s="235"/>
+      <c r="C125" s="226"/>
       <c r="D125" s="154"/>
       <c r="E125" s="154"/>
       <c r="F125" s="154"/>
@@ -5923,8 +5923,8 @@
       <c r="M125" s="4"/>
     </row>
     <row r="126" spans="2:13" ht="18">
-      <c r="B126" s="234"/>
-      <c r="C126" s="231"/>
+      <c r="B126" s="235"/>
+      <c r="C126" s="226"/>
       <c r="D126" s="120"/>
       <c r="E126" s="120"/>
       <c r="F126" s="120"/>
@@ -5937,8 +5937,8 @@
       <c r="M126" s="7"/>
     </row>
     <row r="127" spans="2:13" ht="18">
-      <c r="B127" s="234"/>
-      <c r="C127" s="231"/>
+      <c r="B127" s="235"/>
+      <c r="C127" s="226"/>
       <c r="D127" s="154"/>
       <c r="E127" s="154"/>
       <c r="F127" s="154"/>
@@ -5951,8 +5951,8 @@
       <c r="M127" s="7"/>
     </row>
     <row r="128" spans="2:13" ht="18">
-      <c r="B128" s="234"/>
-      <c r="C128" s="231"/>
+      <c r="B128" s="235"/>
+      <c r="C128" s="226"/>
       <c r="D128" s="120"/>
       <c r="E128" s="120"/>
       <c r="F128" s="120"/>
@@ -5965,8 +5965,8 @@
       <c r="M128" s="7"/>
     </row>
     <row r="129" spans="2:13" ht="18">
-      <c r="B129" s="234"/>
-      <c r="C129" s="231"/>
+      <c r="B129" s="235"/>
+      <c r="C129" s="226"/>
       <c r="D129" s="120"/>
       <c r="E129" s="120"/>
       <c r="F129" s="120"/>
@@ -5979,8 +5979,8 @@
       <c r="M129" s="6"/>
     </row>
     <row r="130" spans="2:13" ht="18">
-      <c r="B130" s="234"/>
-      <c r="C130" s="231"/>
+      <c r="B130" s="235"/>
+      <c r="C130" s="226"/>
       <c r="D130" s="120"/>
       <c r="E130" s="120"/>
       <c r="F130" s="120"/>
@@ -5993,8 +5993,8 @@
       <c r="M130" s="4"/>
     </row>
     <row r="131" spans="2:13" ht="18">
-      <c r="B131" s="234"/>
-      <c r="C131" s="231"/>
+      <c r="B131" s="235"/>
+      <c r="C131" s="226"/>
       <c r="D131" s="120"/>
       <c r="E131" s="120"/>
       <c r="F131" s="120"/>
@@ -6007,8 +6007,8 @@
       <c r="M131" s="4"/>
     </row>
     <row r="132" spans="2:13" ht="18">
-      <c r="B132" s="234"/>
-      <c r="C132" s="231"/>
+      <c r="B132" s="235"/>
+      <c r="C132" s="226"/>
       <c r="D132" s="120"/>
       <c r="E132" s="120"/>
       <c r="F132" s="120"/>
@@ -6021,8 +6021,8 @@
       <c r="M132" s="4"/>
     </row>
     <row r="133" spans="2:13" ht="18">
-      <c r="B133" s="234"/>
-      <c r="C133" s="231"/>
+      <c r="B133" s="235"/>
+      <c r="C133" s="226"/>
       <c r="D133" s="120"/>
       <c r="E133" s="120"/>
       <c r="F133" s="120"/>
@@ -6035,8 +6035,8 @@
       <c r="M133" s="4"/>
     </row>
     <row r="134" spans="2:13" ht="18">
-      <c r="B134" s="234"/>
-      <c r="C134" s="231"/>
+      <c r="B134" s="235"/>
+      <c r="C134" s="226"/>
       <c r="D134" s="120"/>
       <c r="E134" s="120"/>
       <c r="F134" s="120"/>
@@ -6049,8 +6049,8 @@
       <c r="M134" s="4"/>
     </row>
     <row r="135" spans="2:13" ht="18">
-      <c r="B135" s="234"/>
-      <c r="C135" s="231"/>
+      <c r="B135" s="235"/>
+      <c r="C135" s="226"/>
       <c r="D135" s="154"/>
       <c r="E135" s="154"/>
       <c r="F135" s="154"/>
@@ -6063,8 +6063,8 @@
       <c r="M135" s="10"/>
     </row>
     <row r="136" spans="2:13" ht="18">
-      <c r="B136" s="234"/>
-      <c r="C136" s="231"/>
+      <c r="B136" s="235"/>
+      <c r="C136" s="226"/>
       <c r="D136" s="105"/>
       <c r="E136" s="105"/>
       <c r="F136" s="105"/>
@@ -6077,8 +6077,8 @@
       <c r="M136" s="6"/>
     </row>
     <row r="137" spans="2:13" ht="18">
-      <c r="B137" s="236"/>
-      <c r="C137" s="232"/>
+      <c r="B137" s="237"/>
+      <c r="C137" s="227"/>
       <c r="D137" s="108"/>
       <c r="E137" s="108"/>
       <c r="F137" s="109"/>
@@ -6091,8 +6091,8 @@
       <c r="M137" s="2"/>
     </row>
     <row r="138" spans="2:13" ht="18">
-      <c r="B138" s="233"/>
-      <c r="C138" s="225"/>
+      <c r="B138" s="234"/>
+      <c r="C138" s="228"/>
       <c r="D138" s="133"/>
       <c r="E138" s="112"/>
       <c r="F138" s="95"/>
@@ -6105,8 +6105,8 @@
       <c r="M138" s="3"/>
     </row>
     <row r="139" spans="2:13" ht="18">
-      <c r="B139" s="234"/>
-      <c r="C139" s="226"/>
+      <c r="B139" s="235"/>
+      <c r="C139" s="229"/>
       <c r="D139" s="120"/>
       <c r="E139" s="120"/>
       <c r="F139" s="120"/>
@@ -6119,8 +6119,8 @@
       <c r="M139" s="3"/>
     </row>
     <row r="140" spans="2:13" ht="18">
-      <c r="B140" s="234"/>
-      <c r="C140" s="226"/>
+      <c r="B140" s="235"/>
+      <c r="C140" s="229"/>
       <c r="D140" s="120"/>
       <c r="E140" s="120"/>
       <c r="F140" s="120"/>
@@ -6133,8 +6133,8 @@
       <c r="M140" s="3"/>
     </row>
     <row r="141" spans="2:13" ht="18">
-      <c r="B141" s="234"/>
-      <c r="C141" s="226"/>
+      <c r="B141" s="235"/>
+      <c r="C141" s="229"/>
       <c r="D141" s="120"/>
       <c r="E141" s="120"/>
       <c r="F141" s="120"/>
@@ -6147,8 +6147,8 @@
       <c r="M141" s="3"/>
     </row>
     <row r="142" spans="2:13" ht="18">
-      <c r="B142" s="234"/>
-      <c r="C142" s="226"/>
+      <c r="B142" s="235"/>
+      <c r="C142" s="229"/>
       <c r="D142" s="154"/>
       <c r="E142" s="154"/>
       <c r="F142" s="154"/>
@@ -6161,8 +6161,8 @@
       <c r="M142" s="4"/>
     </row>
     <row r="143" spans="2:13" ht="18">
-      <c r="B143" s="234"/>
-      <c r="C143" s="226"/>
+      <c r="B143" s="235"/>
+      <c r="C143" s="229"/>
       <c r="D143" s="120">
         <v>999999999</v>
       </c>
@@ -6177,8 +6177,8 @@
       <c r="M143" s="3"/>
     </row>
     <row r="144" spans="2:13" ht="18">
-      <c r="B144" s="234"/>
-      <c r="C144" s="226"/>
+      <c r="B144" s="235"/>
+      <c r="C144" s="229"/>
       <c r="D144" s="154"/>
       <c r="E144" s="154"/>
       <c r="F144" s="154"/>
@@ -6191,8 +6191,8 @@
       <c r="M144" s="4"/>
     </row>
     <row r="145" spans="2:13" ht="18">
-      <c r="B145" s="234"/>
-      <c r="C145" s="226"/>
+      <c r="B145" s="235"/>
+      <c r="C145" s="229"/>
       <c r="D145" s="120"/>
       <c r="E145" s="120"/>
       <c r="F145" s="120"/>
@@ -6205,8 +6205,8 @@
       <c r="M145" s="3"/>
     </row>
     <row r="146" spans="2:13" ht="18">
-      <c r="B146" s="234"/>
-      <c r="C146" s="226"/>
+      <c r="B146" s="235"/>
+      <c r="C146" s="229"/>
       <c r="D146" s="120"/>
       <c r="E146" s="120"/>
       <c r="F146" s="120"/>
@@ -6219,8 +6219,8 @@
       <c r="M146" s="3"/>
     </row>
     <row r="147" spans="2:13" ht="18">
-      <c r="B147" s="234"/>
-      <c r="C147" s="226"/>
+      <c r="B147" s="235"/>
+      <c r="C147" s="229"/>
       <c r="D147" s="120"/>
       <c r="E147" s="120"/>
       <c r="F147" s="120"/>
@@ -6233,8 +6233,8 @@
       <c r="M147" s="3"/>
     </row>
     <row r="148" spans="2:13" ht="18">
-      <c r="B148" s="234"/>
-      <c r="C148" s="226"/>
+      <c r="B148" s="235"/>
+      <c r="C148" s="229"/>
       <c r="D148" s="120"/>
       <c r="E148" s="120"/>
       <c r="F148" s="120"/>
@@ -6247,8 +6247,8 @@
       <c r="M148" s="3"/>
     </row>
     <row r="149" spans="2:13" ht="18">
-      <c r="B149" s="234"/>
-      <c r="C149" s="226"/>
+      <c r="B149" s="235"/>
+      <c r="C149" s="229"/>
       <c r="D149" s="120"/>
       <c r="E149" s="120"/>
       <c r="F149" s="120"/>
@@ -6261,8 +6261,8 @@
       <c r="M149" s="3"/>
     </row>
     <row r="150" spans="2:13" ht="18">
-      <c r="B150" s="234"/>
-      <c r="C150" s="226"/>
+      <c r="B150" s="235"/>
+      <c r="C150" s="229"/>
       <c r="D150" s="120"/>
       <c r="E150" s="120"/>
       <c r="F150" s="120"/>
@@ -6275,8 +6275,8 @@
       <c r="M150" s="3"/>
     </row>
     <row r="151" spans="2:13" ht="18">
-      <c r="B151" s="234"/>
-      <c r="C151" s="226"/>
+      <c r="B151" s="235"/>
+      <c r="C151" s="229"/>
       <c r="D151" s="120"/>
       <c r="E151" s="120"/>
       <c r="F151" s="120"/>
@@ -6289,8 +6289,8 @@
       <c r="M151" s="3"/>
     </row>
     <row r="152" spans="2:13" ht="18">
-      <c r="B152" s="234"/>
-      <c r="C152" s="226"/>
+      <c r="B152" s="235"/>
+      <c r="C152" s="229"/>
       <c r="D152" s="154"/>
       <c r="E152" s="154"/>
       <c r="F152" s="154"/>
@@ -6303,8 +6303,8 @@
       <c r="M152" s="3"/>
     </row>
     <row r="153" spans="2:13" ht="18">
-      <c r="B153" s="234"/>
-      <c r="C153" s="226"/>
+      <c r="B153" s="235"/>
+      <c r="C153" s="229"/>
       <c r="D153" s="105"/>
       <c r="E153" s="105"/>
       <c r="F153" s="105"/>
@@ -6317,8 +6317,8 @@
       <c r="M153" s="2"/>
     </row>
     <row r="154" spans="2:13" ht="18">
-      <c r="B154" s="234"/>
-      <c r="C154" s="227"/>
+      <c r="B154" s="235"/>
+      <c r="C154" s="230"/>
       <c r="D154" s="108"/>
       <c r="E154" s="108"/>
       <c r="F154" s="109"/>
@@ -6331,7 +6331,7 @@
       <c r="M154" s="2"/>
     </row>
     <row r="155" spans="2:13" ht="19" customHeight="1">
-      <c r="B155" s="228" t="s">
+      <c r="B155" s="231" t="s">
         <v>171</v>
       </c>
       <c r="C155" s="136">
@@ -6368,7 +6368,7 @@
       </c>
     </row>
     <row r="156" spans="2:13" ht="19">
-      <c r="B156" s="228"/>
+      <c r="B156" s="231"/>
       <c r="C156" s="136">
         <v>2</v>
       </c>
@@ -6403,7 +6403,7 @@
       </c>
     </row>
     <row r="157" spans="2:13" ht="20" thickBot="1">
-      <c r="B157" s="228"/>
+      <c r="B157" s="231"/>
       <c r="C157" s="136">
         <v>3</v>
       </c>
@@ -6438,7 +6438,7 @@
       </c>
     </row>
     <row r="158" spans="2:13" ht="21" thickBot="1">
-      <c r="B158" s="228"/>
+      <c r="B158" s="231"/>
       <c r="C158" s="136">
         <v>4</v>
       </c>
@@ -6468,7 +6468,7 @@
       </c>
     </row>
     <row r="159" spans="2:13" ht="33" thickBot="1">
-      <c r="B159" s="228"/>
+      <c r="B159" s="231"/>
       <c r="C159" s="136">
         <v>5</v>
       </c>
@@ -6499,7 +6499,7 @@
       </c>
     </row>
     <row r="160" spans="2:13" ht="33" thickBot="1">
-      <c r="B160" s="228"/>
+      <c r="B160" s="231"/>
       <c r="C160" s="136">
         <v>6</v>
       </c>
@@ -6527,7 +6527,7 @@
       </c>
     </row>
     <row r="161" spans="2:13" ht="33" thickBot="1">
-      <c r="B161" s="228"/>
+      <c r="B161" s="231"/>
       <c r="C161" s="136">
         <v>7</v>
       </c>
@@ -6564,7 +6564,7 @@
       </c>
     </row>
     <row r="162" spans="2:13" ht="32">
-      <c r="B162" s="229"/>
+      <c r="B162" s="232"/>
       <c r="C162" s="171">
         <v>8</v>
       </c>
@@ -6634,11 +6634,15 @@
       </c>
     </row>
     <row r="167" spans="2:13">
+      <c r="D167" s="5">
+        <v>2222</v>
+      </c>
       <c r="I167" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:M162" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="17">
+    <mergeCell ref="B121:B137"/>
     <mergeCell ref="C121:C137"/>
     <mergeCell ref="C138:C154"/>
     <mergeCell ref="B155:B162"/>
@@ -6655,7 +6659,6 @@
     <mergeCell ref="B88:B107"/>
     <mergeCell ref="B108:B120"/>
     <mergeCell ref="C108:C120"/>
-    <mergeCell ref="B121:B137"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>